<commit_message>
Atualização do caso de uso UC-06
</commit_message>
<xml_diff>
--- a/Software para Deficientes Visuais/Casos De Uso/Relacao_Casos_de_Uso.xlsx
+++ b/Software para Deficientes Visuais/Casos De Uso/Relacao_Casos_de_Uso.xlsx
@@ -232,6 +232,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -241,7 +242,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -525,7 +525,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,32 +538,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="7"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="8"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="5" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Casos de Uso, Casos de Teste e Diagrama_Caso_de_Uso.mdj
</commit_message>
<xml_diff>
--- a/Software para Deficientes Visuais/Casos De Uso/Relacao_Casos_de_Uso.xlsx
+++ b/Software para Deficientes Visuais/Casos De Uso/Relacao_Casos_de_Uso.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="39">
   <si>
     <t>Casos de Uso</t>
   </si>
@@ -117,13 +117,37 @@
   </si>
   <si>
     <t>Utilizar o Espaço do Aluno</t>
+  </si>
+  <si>
+    <t>Pendente Evaldo</t>
+  </si>
+  <si>
+    <t>UC-10</t>
+  </si>
+  <si>
+    <t>Uso do DOSVox para leitura de arquivos no formato texto</t>
+  </si>
+  <si>
+    <t>Plano de Testes</t>
+  </si>
+  <si>
+    <t>Rapahel Luz/Rodrigo</t>
+  </si>
+  <si>
+    <t>Raphael</t>
+  </si>
+  <si>
+    <t>Rodrigo</t>
+  </si>
+  <si>
+    <t>Evaldo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,6 +171,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -156,7 +188,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -184,9 +216,7 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -195,22 +225,7 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -220,7 +235,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -232,14 +247,24 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -522,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,41 +558,46 @@
     <col min="1" max="1" width="7" customWidth="1"/>
     <col min="2" max="2" width="69.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" customWidth="1"/>
     <col min="5" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="8"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -587,8 +617,11 @@
         <f>E3</f>
         <v>42916</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -596,7 +629,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>21</v>
@@ -607,8 +640,11 @@
       <c r="F4" s="4">
         <v>42963</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -628,8 +664,11 @@
         <f>E5</f>
         <v>42916</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -649,8 +688,11 @@
         <f>E6</f>
         <v>42916</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -658,7 +700,7 @@
         <v>28</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>21</v>
@@ -666,9 +708,14 @@
       <c r="E7" s="4">
         <v>42969</v>
       </c>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7" s="4">
+        <v>42969</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -676,7 +723,7 @@
         <v>12</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>22</v>
@@ -684,27 +731,37 @@
       <c r="E8" s="4">
         <v>42970</v>
       </c>
-      <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="F8" s="4">
+        <v>42970</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="10">
         <v>42970</v>
       </c>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F9" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>25</v>
       </c>
@@ -723,8 +780,11 @@
       <c r="F10" s="4">
         <v>42963</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>29</v>
       </c>
@@ -732,7 +792,7 @@
         <v>30</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>27</v>
@@ -740,118 +800,84 @@
       <c r="E11" s="4">
         <v>42970</v>
       </c>
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
+      <c r="F11" s="4">
+        <v>42970</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="4">
+        <v>42977</v>
+      </c>
+      <c r="F12" s="4">
+        <v>42977</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
+    </row>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
+    </row>
+    <row r="21" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
+    </row>
+    <row r="22" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E26" s="1"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E27" s="1"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E28" s="1"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E29" s="1"/>
     </row>
   </sheetData>
   <sortState ref="A1:B7">
     <sortCondition ref="A2"/>
   </sortState>
   <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Controle do Plano de Testes. Caso de Testes CT-08
</commit_message>
<xml_diff>
--- a/Software para Deficientes Visuais/Casos De Uso/Relacao_Casos_de_Uso.xlsx
+++ b/Software para Deficientes Visuais/Casos De Uso/Relacao_Casos_de_Uso.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="39">
   <si>
     <t>Casos de Uso</t>
   </si>
@@ -235,7 +235,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -248,12 +248,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -266,6 +260,39 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -547,67 +574,78 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7" customWidth="1"/>
-    <col min="2" max="2" width="69.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" customWidth="1"/>
-    <col min="5" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.42578125" customWidth="1"/>
+    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+    <col min="7" max="7" width="11" customWidth="1"/>
+    <col min="8" max="8" width="11" style="12" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+    </row>
+    <row r="2" spans="1:9" s="21" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="20" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="14" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="17" t="s">
         <v>20</v>
       </c>
       <c r="E3" s="4">
@@ -620,18 +658,22 @@
       <c r="G3" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="11">
+        <v>42984</v>
+      </c>
+      <c r="I3" s="13"/>
+    </row>
+    <row r="4" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="14" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="17" t="s">
         <v>21</v>
       </c>
       <c r="E4" s="4">
@@ -643,18 +685,22 @@
       <c r="G4" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="11">
+        <v>42984</v>
+      </c>
+      <c r="I4" s="13"/>
+    </row>
+    <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="14" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="17" t="s">
         <v>20</v>
       </c>
       <c r="E5" s="4">
@@ -667,18 +713,22 @@
       <c r="G5" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="11">
+        <v>42984</v>
+      </c>
+      <c r="I5" s="13"/>
+    </row>
+    <row r="6" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="17" t="s">
         <v>20</v>
       </c>
       <c r="E6" s="4">
@@ -691,18 +741,22 @@
       <c r="G6" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="11">
+        <v>42984</v>
+      </c>
+      <c r="I6" s="13"/>
+    </row>
+    <row r="7" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="14" t="s">
         <v>28</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="17" t="s">
         <v>21</v>
       </c>
       <c r="E7" s="4">
@@ -714,18 +768,22 @@
       <c r="G7" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="11">
+        <v>42984</v>
+      </c>
+      <c r="I7" s="13"/>
+    </row>
+    <row r="8" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="14" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="17" t="s">
         <v>22</v>
       </c>
       <c r="E8" s="4">
@@ -737,41 +795,49 @@
       <c r="G8" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="H8" s="11">
+        <v>42984</v>
+      </c>
+      <c r="I8" s="13"/>
+    </row>
+    <row r="9" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="8">
         <v>42970</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="6" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" s="11">
+        <v>42984</v>
+      </c>
+      <c r="I9" s="13"/>
+    </row>
+    <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="14" t="s">
         <v>26</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="17" t="s">
         <v>27</v>
       </c>
       <c r="E10" s="4">
@@ -783,18 +849,24 @@
       <c r="G10" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10" s="11">
+        <v>42984</v>
+      </c>
+      <c r="I10" s="11">
+        <v>42984</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="14" t="s">
         <v>30</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="17" t="s">
         <v>27</v>
       </c>
       <c r="E11" s="4">
@@ -806,18 +878,22 @@
       <c r="G11" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" s="11">
+        <v>42984</v>
+      </c>
+      <c r="I11" s="13"/>
+    </row>
+    <row r="12" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="16" t="s">
         <v>33</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="17" t="s">
         <v>35</v>
       </c>
       <c r="E12" s="4">
@@ -829,47 +905,51 @@
       <c r="G12" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" s="11">
+        <v>42984</v>
+      </c>
+      <c r="I12" s="13"/>
+    </row>
+    <row r="13" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="5:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="5:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="5:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="5:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E22" s="1"/>
     </row>
   </sheetData>
@@ -877,7 +957,7 @@
     <sortCondition ref="A2"/>
   </sortState>
   <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A1:I1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualização do diagrama e casos de teste
</commit_message>
<xml_diff>
--- a/Software para Deficientes Visuais/Casos De Uso/Relacao_Casos_de_Uso.xlsx
+++ b/Software para Deficientes Visuais/Casos De Uso/Relacao_Casos_de_Uso.xlsx
@@ -235,7 +235,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -247,7 +247,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -255,43 +254,50 @@
     <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -589,49 +595,49 @@
     <col min="5" max="5" width="11.5703125" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="8" max="8" width="11" style="12" customWidth="1"/>
+    <col min="8" max="8" width="11" style="9" customWidth="1"/>
     <col min="9" max="9" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-    </row>
-    <row r="2" spans="1:9" s="21" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+    </row>
+    <row r="2" spans="1:9" s="17" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="16" t="s">
         <v>34</v>
       </c>
     </row>
@@ -639,13 +645,13 @@
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="11" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="13" t="s">
         <v>20</v>
       </c>
       <c r="E3" s="4">
@@ -658,77 +664,79 @@
       <c r="G3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H3" s="11">
-        <v>42984</v>
-      </c>
-      <c r="I3" s="13"/>
+      <c r="H3" s="8">
+        <v>42984</v>
+      </c>
+      <c r="I3" s="8">
+        <v>42984</v>
+      </c>
     </row>
     <row r="4" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="7">
         <v>42963</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="7">
         <v>42963</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="11">
-        <v>42984</v>
-      </c>
-      <c r="I4" s="13"/>
+      <c r="H4" s="20">
+        <v>42991</v>
+      </c>
+      <c r="I4" s="21"/>
     </row>
     <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="7">
         <v>42916</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="7">
         <f>E5</f>
         <v>42916</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="11">
-        <v>42984</v>
-      </c>
-      <c r="I5" s="13"/>
+      <c r="H5" s="20">
+        <v>42991</v>
+      </c>
+      <c r="I5" s="21"/>
     </row>
     <row r="6" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="11" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="13" t="s">
         <v>20</v>
       </c>
       <c r="E6" s="4">
@@ -741,49 +749,51 @@
       <c r="G6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="11">
-        <v>42984</v>
-      </c>
-      <c r="I6" s="13"/>
+      <c r="H6" s="8">
+        <v>42984</v>
+      </c>
+      <c r="I6" s="8">
+        <v>42984</v>
+      </c>
     </row>
     <row r="7" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="7">
         <v>42969</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="7">
         <v>42969</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="11">
-        <v>42984</v>
-      </c>
-      <c r="I7" s="13"/>
+      <c r="H7" s="20">
+        <v>42991</v>
+      </c>
+      <c r="I7" s="21"/>
     </row>
     <row r="8" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="11" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="13" t="s">
         <v>22</v>
       </c>
       <c r="E8" s="4">
@@ -795,49 +805,51 @@
       <c r="G8" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H8" s="11">
-        <v>42984</v>
-      </c>
-      <c r="I8" s="13"/>
+      <c r="H8" s="8">
+        <v>42984</v>
+      </c>
+      <c r="I8" s="8">
+        <v>42984</v>
+      </c>
     </row>
     <row r="9" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="7">
         <v>42970</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="11">
-        <v>42984</v>
-      </c>
-      <c r="I9" s="13"/>
+      <c r="H9" s="8">
+        <v>42984</v>
+      </c>
+      <c r="I9" s="10"/>
     </row>
     <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="11" t="s">
         <v>26</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="13" t="s">
         <v>27</v>
       </c>
       <c r="E10" s="4">
@@ -849,10 +861,10 @@
       <c r="G10" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="H10" s="11">
-        <v>42984</v>
-      </c>
-      <c r="I10" s="11">
+      <c r="H10" s="8">
+        <v>42984</v>
+      </c>
+      <c r="I10" s="8">
         <v>42984</v>
       </c>
     </row>
@@ -860,13 +872,13 @@
       <c r="A11" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="11" t="s">
         <v>30</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="13" t="s">
         <v>27</v>
       </c>
       <c r="E11" s="4">
@@ -878,37 +890,39 @@
       <c r="G11" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="H11" s="11">
-        <v>42984</v>
-      </c>
-      <c r="I11" s="13"/>
+      <c r="H11" s="8">
+        <v>42984</v>
+      </c>
+      <c r="I11" s="8">
+        <v>42984</v>
+      </c>
     </row>
     <row r="12" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="7">
         <v>42977</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="7">
         <v>42977</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="H12" s="11">
-        <v>42984</v>
-      </c>
-      <c r="I12" s="13"/>
+      <c r="H12" s="20">
+        <v>42991</v>
+      </c>
+      <c r="I12" s="21"/>
     </row>
     <row r="13" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="1"/>

</xml_diff>